<commit_message>
Update on slides & schedule
</commit_message>
<xml_diff>
--- a/Project Schedule & Tasks Allocation.xlsx
+++ b/Project Schedule & Tasks Allocation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b9b2384c46af58b4/Datasci/GA/DSI 12 Work Area/classes/Project1234/project_4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dfait\OneDrive\Datasci\GA\DSI 12 Work Area\classes\Project1234\Project_4_Grp\dsi12_proj4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E00B912F-9687-43E8-BBCC-71A6468070EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{E00B912F-9687-43E8-BBCC-71A6468070EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2255406-E4ED-4833-9590-BEA9F6CEB59A}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{D59C134F-96DC-4980-8E77-E0117380945A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>Task</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Boon Jun, Sathya</t>
-  </si>
-  <si>
-    <t>Wesley, Russell, Boon Jun</t>
   </si>
   <si>
     <t>Tasks Allocation</t>
@@ -683,7 +680,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -724,7 +721,7 @@
     </row>
     <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>22</v>
@@ -903,7 +900,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -917,7 +914,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>